<commit_message>
Update the mapping predicates list
</commit_message>
<xml_diff>
--- a/crosswalks/templates/classifier-crosswalk-sssom-template.xlsx
+++ b/crosswalks/templates/classifier-crosswalk-sssom-template.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ecosystem-typology\crosswalks\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0990EFB-7B57-40B6-88F3-E25A8505C84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F12595-6C61-4FA7-958D-DE709A653CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3660" windowWidth="38310" windowHeight="14295" activeTab="2" xr2:uid="{00E2F0C7-36F4-48CD-AB7C-87DDD7B41E94}"/>
+    <workbookView xWindow="8970" yWindow="3090" windowWidth="26955" windowHeight="14295" activeTab="4" xr2:uid="{00E2F0C7-36F4-48CD-AB7C-87DDD7B41E94}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <sheet name="justification" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -176,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="230">
   <si>
     <t>subject_id</t>
   </si>
@@ -857,13 +856,22 @@
   </si>
   <si>
     <t>Good</t>
+  </si>
+  <si>
+    <t>skos:relatedMatch</t>
+  </si>
+  <si>
+    <t>skos:mappingRelation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this when the target of the mapping is 'owl:Nothing' </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,12 +884,6 @@
       <sz val="9"/>
       <color rgb="FF1F2328"/>
       <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -926,7 +928,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1348,27 +1350,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A7C4E4-783A-4F29-A8C4-C75B03DD1963}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="41.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1417,7 +1420,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" promptTitle="predicates" prompt="Select mapping predicate" xr:uid="{B242DDBD-390B-4491-9671-2CBFE699378F}">
           <x14:formula1>
-            <xm:f>predicate_id!$A$1:$A$4</xm:f>
+            <xm:f>predicate_id!$A$1:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>C1:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -1441,13 +1444,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBAACB4D-58E5-4DBA-B465-4D3098E5C8AD}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.7109375" customWidth="1"/>
+    <col min="1" max="1" width="72.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1507,28 +1513,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA42FDB6-D150-40A8-8A7A-07EE71241144}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" customWidth="1"/>
-    <col min="6" max="6" width="33" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" customWidth="1"/>
-    <col min="11" max="11" width="41.7109375" customWidth="1"/>
-    <col min="12" max="12" width="36" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1866,15 +1873,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2293BD-1F16-4B7C-9AFD-82E79329438B}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A10"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="104.140625" customWidth="1"/>
+    <col min="1" max="1" width="95.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1929,37 +1937,55 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E30729-B883-4977-BF99-5B48A44F48C2}">
-  <dimension ref="A1:A4"/>
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -1969,10 +1995,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858F67D3-E433-4504-A92A-4AAB7DEB3195}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:XFD3"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2009,21 +2036,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441A2E52-8546-4786-A1BE-7FFC67B91F3B}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="218.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="172" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="72.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>